<commit_message>
fix buf ve gantt chi mot doan
</commit_message>
<xml_diff>
--- a/inputdata.xlsx
+++ b/inputdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Name" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name of worker</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Gỡ + Check Coating</t>
+  </si>
+  <si>
+    <t>Hàn gá</t>
+  </si>
+  <si>
+    <t>Hàn full</t>
+  </si>
+  <si>
+    <t>Hạnh</t>
   </si>
 </sst>
 </file>
@@ -451,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,6 +511,11 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -513,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +592,12 @@
       <c r="B6" t="s">
         <v>18</v>
       </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
fix bug hien thi
</commit_message>
<xml_diff>
--- a/inputdata.xlsx
+++ b/inputdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Name" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name of worker</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Hạnh</t>
+  </si>
+  <si>
+    <t>Vệ sinh</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -527,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +601,9 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>